<commit_message>
Tiedosto johon tuotu siivottu lopputulos.
</commit_message>
<xml_diff>
--- a/Data/Data-clean.xlsx
+++ b/Data/Data-clean.xlsx
@@ -1,37 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1360" yWindow="260" windowWidth="21600" windowHeight="11060" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Taul1" sheetId="1" r:id="rId1"/>
+    <sheet name="Taul1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="15"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,22 +66,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -330,13 +409,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nimi</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Tsekkaus</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Tonttu</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Tämä jää</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>Toljander</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Tämä jää</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Joulupukki</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Tämä jää</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>Muori</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Tämä jää</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="19.5" customHeight="1">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Tämä jää</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Viimeinen commit. Sis. uudelleennimettyjä tiedostoja testiversioista.
</commit_message>
<xml_diff>
--- a/Data/Data-clean.xlsx
+++ b/Data/Data-clean.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1360" yWindow="260" windowWidth="21600" windowHeight="11060" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11175" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" state="visible" r:id="rId1"/>
@@ -414,13 +414,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="18.26953125" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
@@ -433,9 +436,19 @@
           <t>Nimi</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Turha</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Tsekkaus</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uusi </t>
         </is>
       </c>
     </row>
@@ -448,9 +461,19 @@
           <t>Tonttu</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>turhuus</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Tämä jää</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Testaa</t>
         </is>
       </c>
     </row>
@@ -463,9 +486,19 @@
           <t>Toljander</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>turhuus</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>Tämä jää</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>Testaa</t>
         </is>
       </c>
     </row>
@@ -478,9 +511,19 @@
           <t>Joulupukki</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>turhuus</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>Tämä jää</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>Testaa</t>
         </is>
       </c>
     </row>
@@ -493,9 +536,19 @@
           <t>Muori</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>turhuus</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>Tämä jää</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>Testaa</t>
         </is>
       </c>
     </row>
@@ -508,9 +561,19 @@
           <t>Smith</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>turhuus</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>Tämä jää</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>Testaa</t>
         </is>
       </c>
     </row>

</xml_diff>